<commit_message>
Atualização 20 e 21/06
</commit_message>
<xml_diff>
--- a/Sergipe/output/historico_sergipe.xlsx
+++ b/Sergipe/output/historico_sergipe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/DataViz/covid19-br/Vacinacao/Sergipe/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA58103F-1D99-DC4B-865E-62037DE7497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A25F42-03FB-9B46-A6F9-6E1DC2AA5665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19080" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2175,6 +2175,40 @@
         <v>219085</v>
       </c>
     </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="2">
+        <v>44367</v>
+      </c>
+      <c r="B102">
+        <v>734997</v>
+      </c>
+      <c r="C102">
+        <v>694462</v>
+      </c>
+      <c r="D102">
+        <v>270813</v>
+      </c>
+      <c r="E102">
+        <v>219138</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="2">
+        <v>44368</v>
+      </c>
+      <c r="B103">
+        <v>734847</v>
+      </c>
+      <c r="C103">
+        <v>716309</v>
+      </c>
+      <c r="D103">
+        <v>270813</v>
+      </c>
+      <c r="E103">
+        <v>219298</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização 29/06 com dados da dose única
</commit_message>
<xml_diff>
--- a/Sergipe/output/historico_sergipe.xlsx
+++ b/Sergipe/output/historico_sergipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/DataViz/covid19-br/Vacinacao/Sergipe/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED57BFB0-3CC0-784C-AF7B-127E327C1CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CED46C-7EDE-0F44-8D66-D43254C9CDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19080" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>data</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>aplicadas_dose2</t>
+  </si>
+  <si>
+    <t>enviadas_dose_unica</t>
+  </si>
+  <si>
+    <t>aplicadas_dose_unica</t>
   </si>
 </sst>
 </file>
@@ -69,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -92,17 +98,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -443,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -458,7 +481,7 @@
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,8 +497,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44256</v>
       </c>
@@ -491,8 +520,14 @@
       <c r="E2" s="3">
         <v>24909</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44257</v>
       </c>
@@ -508,8 +543,14 @@
       <c r="E3" s="3">
         <v>25744</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44258</v>
       </c>
@@ -525,8 +566,14 @@
       <c r="E4" s="3">
         <v>26816</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44259</v>
       </c>
@@ -542,8 +589,14 @@
       <c r="E5" s="3">
         <v>27275</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44260</v>
       </c>
@@ -559,8 +612,14 @@
       <c r="E6" s="3">
         <v>28353</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44263</v>
       </c>
@@ -576,8 +635,14 @@
       <c r="E7" s="3">
         <v>29357</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44264</v>
       </c>
@@ -593,8 +658,14 @@
       <c r="E8" s="3">
         <v>30199</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44265</v>
       </c>
@@ -610,8 +681,14 @@
       <c r="E9" s="3">
         <v>30724</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44266</v>
       </c>
@@ -627,8 +704,14 @@
       <c r="E10">
         <v>31583</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44267</v>
       </c>
@@ -644,8 +727,14 @@
       <c r="E11">
         <v>31944</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44270</v>
       </c>
@@ -661,8 +750,14 @@
       <c r="E12">
         <v>32665</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44271</v>
       </c>
@@ -678,8 +773,14 @@
       <c r="E13">
         <v>33355</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44272</v>
       </c>
@@ -695,8 +796,14 @@
       <c r="E14">
         <v>34748</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44273</v>
       </c>
@@ -712,8 +819,14 @@
       <c r="E15">
         <v>34748</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44274</v>
       </c>
@@ -729,8 +842,14 @@
       <c r="E16">
         <v>34748</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44276</v>
       </c>
@@ -746,8 +865,14 @@
       <c r="E17">
         <v>34748</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44277</v>
       </c>
@@ -763,8 +888,14 @@
       <c r="E18">
         <v>34453</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44278</v>
       </c>
@@ -780,8 +911,14 @@
       <c r="E19">
         <v>35515</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44279</v>
       </c>
@@ -797,8 +934,14 @@
       <c r="E20">
         <v>37237</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44280</v>
       </c>
@@ -814,8 +957,14 @@
       <c r="E21">
         <v>39552</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44281</v>
       </c>
@@ -831,8 +980,14 @@
       <c r="E22">
         <v>40811</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="5">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44282</v>
       </c>
@@ -848,8 +1003,14 @@
       <c r="E23">
         <v>41819</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44284</v>
       </c>
@@ -865,8 +1026,14 @@
       <c r="E24">
         <v>43141</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44285</v>
       </c>
@@ -882,8 +1049,14 @@
       <c r="E25">
         <v>45157</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44286</v>
       </c>
@@ -899,8 +1072,14 @@
       <c r="E26">
         <v>48618</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44287</v>
       </c>
@@ -916,8 +1095,14 @@
       <c r="E27">
         <v>49356</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44288</v>
       </c>
@@ -933,8 +1118,14 @@
       <c r="E28">
         <v>51191</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44289</v>
       </c>
@@ -950,8 +1141,14 @@
       <c r="E29">
         <v>52238</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44290</v>
       </c>
@@ -967,8 +1164,14 @@
       <c r="E30">
         <v>52434</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44291</v>
       </c>
@@ -984,8 +1187,14 @@
       <c r="E31">
         <v>55209</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44292</v>
       </c>
@@ -1001,8 +1210,14 @@
       <c r="E32">
         <v>57346</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44293</v>
       </c>
@@ -1018,8 +1233,14 @@
       <c r="E33">
         <v>59400</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="5">
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44294</v>
       </c>
@@ -1035,8 +1256,14 @@
       <c r="E34">
         <v>60518</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="5">
+        <v>0</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44295</v>
       </c>
@@ -1052,8 +1279,14 @@
       <c r="E35">
         <v>63304</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="5">
+        <v>0</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44296</v>
       </c>
@@ -1069,8 +1302,14 @@
       <c r="E36">
         <v>64115</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44297</v>
       </c>
@@ -1086,8 +1325,14 @@
       <c r="E37">
         <v>64504</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44298</v>
       </c>
@@ -1103,8 +1348,14 @@
       <c r="E38">
         <v>67423</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44299</v>
       </c>
@@ -1120,8 +1371,14 @@
       <c r="E39">
         <v>73632</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44300</v>
       </c>
@@ -1137,8 +1394,14 @@
       <c r="E40">
         <v>78497</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44301</v>
       </c>
@@ -1154,8 +1417,14 @@
       <c r="E41">
         <v>88607</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44302</v>
       </c>
@@ -1171,8 +1440,14 @@
       <c r="E42">
         <v>96335</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="5">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44303</v>
       </c>
@@ -1188,8 +1463,14 @@
       <c r="E43">
         <v>99658</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44304</v>
       </c>
@@ -1205,8 +1486,14 @@
       <c r="E44">
         <v>102373</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44305</v>
       </c>
@@ -1222,8 +1509,14 @@
       <c r="E45">
         <v>106409</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="5">
+        <v>0</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44306</v>
       </c>
@@ -1239,8 +1532,14 @@
       <c r="E46">
         <v>116580</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="5">
+        <v>0</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44307</v>
       </c>
@@ -1256,8 +1555,14 @@
       <c r="E47">
         <v>121645</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="5">
+        <v>0</v>
+      </c>
+      <c r="G47" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44308</v>
       </c>
@@ -1273,8 +1578,14 @@
       <c r="E48">
         <v>128604</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="5">
+        <v>0</v>
+      </c>
+      <c r="G48" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44309</v>
       </c>
@@ -1290,8 +1601,14 @@
       <c r="E49">
         <v>132536</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="5">
+        <v>0</v>
+      </c>
+      <c r="G49" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44310</v>
       </c>
@@ -1307,8 +1624,14 @@
       <c r="E50">
         <v>134221</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="5">
+        <v>0</v>
+      </c>
+      <c r="G50" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44311</v>
       </c>
@@ -1324,8 +1647,14 @@
       <c r="E51">
         <v>134243</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="5">
+        <v>0</v>
+      </c>
+      <c r="G51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44312</v>
       </c>
@@ -1341,8 +1670,14 @@
       <c r="E52">
         <v>136771</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="5">
+        <v>0</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44313</v>
       </c>
@@ -1358,8 +1693,14 @@
       <c r="E53">
         <v>140779</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="5">
+        <v>0</v>
+      </c>
+      <c r="G53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44314</v>
       </c>
@@ -1375,8 +1716,14 @@
       <c r="E54">
         <v>142478</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="5">
+        <v>0</v>
+      </c>
+      <c r="G54" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44315</v>
       </c>
@@ -1392,8 +1739,14 @@
       <c r="E55">
         <v>143434</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="5">
+        <v>0</v>
+      </c>
+      <c r="G55" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44316</v>
       </c>
@@ -1409,8 +1762,14 @@
       <c r="E56">
         <v>144046</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="5">
+        <v>0</v>
+      </c>
+      <c r="G56" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44318</v>
       </c>
@@ -1426,8 +1785,14 @@
       <c r="E57">
         <v>144700</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="5">
+        <v>0</v>
+      </c>
+      <c r="G57" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44319</v>
       </c>
@@ -1443,8 +1808,14 @@
       <c r="E58">
         <v>145450</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="5">
+        <v>0</v>
+      </c>
+      <c r="G58" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44320</v>
       </c>
@@ -1460,8 +1831,14 @@
       <c r="E59">
         <v>147637</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="5">
+        <v>0</v>
+      </c>
+      <c r="G59" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44321</v>
       </c>
@@ -1477,8 +1854,14 @@
       <c r="E60">
         <v>153177</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="5">
+        <v>0</v>
+      </c>
+      <c r="G60" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44322</v>
       </c>
@@ -1494,8 +1877,14 @@
       <c r="E61">
         <v>154060</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="5">
+        <v>0</v>
+      </c>
+      <c r="G61" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44323</v>
       </c>
@@ -1511,8 +1900,14 @@
       <c r="E62">
         <v>155432</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="5">
+        <v>0</v>
+      </c>
+      <c r="G62" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44324</v>
       </c>
@@ -1528,8 +1923,14 @@
       <c r="E63">
         <v>156517</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="5">
+        <v>0</v>
+      </c>
+      <c r="G63" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44326</v>
       </c>
@@ -1545,8 +1946,14 @@
       <c r="E64">
         <v>158954</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="5">
+        <v>0</v>
+      </c>
+      <c r="G64" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44327</v>
       </c>
@@ -1562,8 +1969,14 @@
       <c r="E65">
         <v>160270</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="5">
+        <v>0</v>
+      </c>
+      <c r="G65" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44328</v>
       </c>
@@ -1579,8 +1992,14 @@
       <c r="E66">
         <v>162936</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="5">
+        <v>0</v>
+      </c>
+      <c r="G66" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44329</v>
       </c>
@@ -1596,8 +2015,14 @@
       <c r="E67">
         <v>165173</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="5">
+        <v>0</v>
+      </c>
+      <c r="G67" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44330</v>
       </c>
@@ -1613,8 +2038,14 @@
       <c r="E68">
         <v>166045</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="5">
+        <v>0</v>
+      </c>
+      <c r="G68" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44331</v>
       </c>
@@ -1630,8 +2061,14 @@
       <c r="E69">
         <v>166163</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="5">
+        <v>0</v>
+      </c>
+      <c r="G69" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44332</v>
       </c>
@@ -1647,8 +2084,14 @@
       <c r="E70">
         <v>173677</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="5">
+        <v>0</v>
+      </c>
+      <c r="G70" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44333</v>
       </c>
@@ -1664,8 +2107,14 @@
       <c r="E71">
         <v>175619</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="5">
+        <v>0</v>
+      </c>
+      <c r="G71" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44334</v>
       </c>
@@ -1681,8 +2130,14 @@
       <c r="E72">
         <v>181019</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="5">
+        <v>0</v>
+      </c>
+      <c r="G72" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44335</v>
       </c>
@@ -1698,8 +2153,14 @@
       <c r="E73">
         <v>182639</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="5">
+        <v>0</v>
+      </c>
+      <c r="G73" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44336</v>
       </c>
@@ -1715,8 +2176,14 @@
       <c r="E74">
         <v>184225</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="5">
+        <v>0</v>
+      </c>
+      <c r="G74" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44337</v>
       </c>
@@ -1732,8 +2199,14 @@
       <c r="E75">
         <v>184945</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="5">
+        <v>0</v>
+      </c>
+      <c r="G75" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44338</v>
       </c>
@@ -1749,8 +2222,14 @@
       <c r="E76">
         <v>185353</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="5">
+        <v>0</v>
+      </c>
+      <c r="G76" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44340</v>
       </c>
@@ -1766,8 +2245,14 @@
       <c r="E77">
         <v>185927</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="5">
+        <v>0</v>
+      </c>
+      <c r="G77" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44341</v>
       </c>
@@ -1783,8 +2268,14 @@
       <c r="E78">
         <v>190226</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="5">
+        <v>0</v>
+      </c>
+      <c r="G78" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44342</v>
       </c>
@@ -1800,8 +2291,14 @@
       <c r="E79">
         <v>190692</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="5">
+        <v>0</v>
+      </c>
+      <c r="G79" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44343</v>
       </c>
@@ -1817,8 +2314,14 @@
       <c r="E80">
         <v>191107</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="5">
+        <v>0</v>
+      </c>
+      <c r="G80" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44344</v>
       </c>
@@ -1834,8 +2337,14 @@
       <c r="E81">
         <v>191912</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="5">
+        <v>0</v>
+      </c>
+      <c r="G81" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44345</v>
       </c>
@@ -1851,8 +2360,14 @@
       <c r="E82">
         <v>192410</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="5">
+        <v>0</v>
+      </c>
+      <c r="G82" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44346</v>
       </c>
@@ -1868,8 +2383,14 @@
       <c r="E83">
         <v>193335</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="5">
+        <v>0</v>
+      </c>
+      <c r="G83" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44347</v>
       </c>
@@ -1885,8 +2406,14 @@
       <c r="E84">
         <v>193500</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="5">
+        <v>0</v>
+      </c>
+      <c r="G84" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44348</v>
       </c>
@@ -1902,8 +2429,14 @@
       <c r="E85">
         <v>194161</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="5">
+        <v>0</v>
+      </c>
+      <c r="G85" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44349</v>
       </c>
@@ -1919,8 +2452,14 @@
       <c r="E86">
         <v>196071</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86" s="5">
+        <v>0</v>
+      </c>
+      <c r="G86" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44350</v>
       </c>
@@ -1936,8 +2475,14 @@
       <c r="E87">
         <v>196987</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87" s="5">
+        <v>0</v>
+      </c>
+      <c r="G87" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44351</v>
       </c>
@@ -1953,8 +2498,14 @@
       <c r="E88">
         <v>197634</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88" s="5">
+        <v>0</v>
+      </c>
+      <c r="G88" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44353</v>
       </c>
@@ -1970,8 +2521,14 @@
       <c r="E89">
         <v>198698</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89" s="5">
+        <v>0</v>
+      </c>
+      <c r="G89" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44354</v>
       </c>
@@ -1987,8 +2544,14 @@
       <c r="E90">
         <v>199548</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90" s="5">
+        <v>0</v>
+      </c>
+      <c r="G90" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44355</v>
       </c>
@@ -2004,8 +2567,14 @@
       <c r="E91">
         <v>206729</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91" s="5">
+        <v>0</v>
+      </c>
+      <c r="G91" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44356</v>
       </c>
@@ -2021,8 +2590,14 @@
       <c r="E92">
         <v>208031</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92" s="5">
+        <v>0</v>
+      </c>
+      <c r="G92" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44357</v>
       </c>
@@ -2038,8 +2613,14 @@
       <c r="E93">
         <v>208299</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93" s="5">
+        <v>0</v>
+      </c>
+      <c r="G93" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44358</v>
       </c>
@@ -2055,8 +2636,14 @@
       <c r="E94">
         <v>209600</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94" s="5">
+        <v>0</v>
+      </c>
+      <c r="G94" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44359</v>
       </c>
@@ -2072,8 +2659,14 @@
       <c r="E95">
         <v>210437</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95" s="5">
+        <v>0</v>
+      </c>
+      <c r="G95" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44360</v>
       </c>
@@ -2089,8 +2682,14 @@
       <c r="E96">
         <v>210694</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96" s="5">
+        <v>0</v>
+      </c>
+      <c r="G96" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>44361</v>
       </c>
@@ -2106,8 +2705,14 @@
       <c r="E97">
         <v>210993</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97" s="5">
+        <v>0</v>
+      </c>
+      <c r="G97" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>44362</v>
       </c>
@@ -2123,8 +2728,14 @@
       <c r="E98">
         <v>216942</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98" s="5">
+        <v>0</v>
+      </c>
+      <c r="G98" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>44363</v>
       </c>
@@ -2140,8 +2751,14 @@
       <c r="E99">
         <v>217837</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99" s="5">
+        <v>0</v>
+      </c>
+      <c r="G99" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>44364</v>
       </c>
@@ -2157,8 +2774,14 @@
       <c r="E100">
         <v>218403</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100" s="5">
+        <v>0</v>
+      </c>
+      <c r="G100" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>44365</v>
       </c>
@@ -2174,8 +2797,14 @@
       <c r="E101">
         <v>219085</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101" s="5">
+        <v>0</v>
+      </c>
+      <c r="G101" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>44367</v>
       </c>
@@ -2191,8 +2820,14 @@
       <c r="E102">
         <v>219138</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102" s="5">
+        <v>0</v>
+      </c>
+      <c r="G102" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>44368</v>
       </c>
@@ -2208,8 +2843,14 @@
       <c r="E103">
         <v>219298</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103" s="5">
+        <v>0</v>
+      </c>
+      <c r="G103" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>44369</v>
       </c>
@@ -2225,8 +2866,14 @@
       <c r="E104">
         <v>219991</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104" s="5">
+        <v>0</v>
+      </c>
+      <c r="G104" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>44370</v>
       </c>
@@ -2242,8 +2889,14 @@
       <c r="E105">
         <v>220590</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105" s="5">
+        <v>0</v>
+      </c>
+      <c r="G105" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>44374</v>
       </c>
@@ -2258,6 +2911,58 @@
       </c>
       <c r="E106">
         <v>225871</v>
+      </c>
+      <c r="F106" s="5">
+        <v>0</v>
+      </c>
+      <c r="G106" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
+        <v>44375</v>
+      </c>
+      <c r="B107">
+        <v>791752</v>
+      </c>
+      <c r="C107">
+        <v>761736</v>
+      </c>
+      <c r="D107">
+        <v>270843</v>
+      </c>
+      <c r="E107">
+        <v>233760</v>
+      </c>
+      <c r="F107" s="5">
+        <v>0</v>
+      </c>
+      <c r="G107" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
+        <v>44376</v>
+      </c>
+      <c r="B108">
+        <v>791752</v>
+      </c>
+      <c r="C108">
+        <v>766016</v>
+      </c>
+      <c r="D108">
+        <v>270843</v>
+      </c>
+      <c r="E108">
+        <v>236511</v>
+      </c>
+      <c r="F108" s="5">
+        <v>16300</v>
+      </c>
+      <c r="G108" s="5">
+        <v>9222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>